<commit_message>
Pembarharuan Kode dan Files
</commit_message>
<xml_diff>
--- a/Olah Nilai/4B/Daftar Nilai UAS 4B.xlsx
+++ b/Olah Nilai/4B/Daftar Nilai UAS 4B.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="20490" windowHeight="7620" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -1365,7 +1365,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>6</col>
@@ -1380,21 +1380,21 @@
         <cNvPicPr preferRelativeResize="0"/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="6200775" y="9810750"/>
           <a:ext cx="552450" cy="238125"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1600,7 +1600,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -3549,7 +3549,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" paperSize="9"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
</xml_diff>